<commit_message>
daily status update for 31mar by nitesh
</commit_message>
<xml_diff>
--- a/Daily Status update Report 2803.xlsx
+++ b/Daily Status update Report 2803.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="89">
   <si>
     <t>Employee Name</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Reviewed point discussed of Theoretical Pricing  and reviewed test cases of Clearing DPD</t>
+  </si>
+  <si>
+    <t>Setup of Git; Understanding SLA document for PT</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3054,7 +3057,274 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3216,7 +3486,7 @@
         <v>0.75</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3238,9 +3508,7 @@
       <c r="F11" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>81</v>
-      </c>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
@@ -3261,9 +3529,7 @@
       <c r="F12" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -3284,9 +3550,7 @@
       <c r="F13" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -3310,158 +3574,6 @@
       <c r="G14" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated by nitesh 2 time
</commit_message>
<xml_diff>
--- a/Daily Status update Report 2803.xlsx
+++ b/Daily Status update Report 2803.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="89">
   <si>
     <t>Employee Name</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Reviewed point discussed of Theoretical Pricing  and reviewed test cases of Clearing DPD</t>
+  </si>
+  <si>
+    <t>Setup of Git;Understanding SLA document for PT</t>
   </si>
 </sst>
 </file>
@@ -3054,7 +3057,274 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3216,7 +3486,7 @@
         <v>0.75</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3238,9 +3508,7 @@
       <c r="F11" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>81</v>
-      </c>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
@@ -3261,9 +3529,7 @@
       <c r="F12" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -3284,9 +3550,7 @@
       <c r="F13" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -3310,158 +3574,6 @@
       <c r="G14" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated by adding sheet for 1st april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 2803.xlsx
+++ b/Daily Status update Report 2803.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="27-Mar" sheetId="7" r:id="rId7"/>
     <sheet name="30-Mar" sheetId="8" r:id="rId8"/>
     <sheet name="31-Mar" sheetId="9" r:id="rId9"/>
+    <sheet name="1-Apr" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="89">
   <si>
     <t>Employee Name</t>
   </si>
@@ -691,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1014,6 +1015,264 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3324,8 +3583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>